<commit_message>
Update training with equations
</commit_message>
<xml_diff>
--- a/Assignments/PA4/training.xlsx
+++ b/Assignments/PA4/training.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">File Name</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>dtoh_bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convolution Prediction Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covariance Prediction Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2D Prediction Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2H Prediction Time</t>
   </si>
   <si>
     <t>./600x600_cat.pgm</t>
@@ -130,8 +142,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -175,10 +189,18 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,6 +548,159 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2:$H$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="0"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:txPr>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>2160000</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>3840000</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>11760000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>15360000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>19440000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>29040000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>34560000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>40560000</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>47040000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>54000000</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>69360000</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>77760000</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>86640000</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>105840000</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>126960000</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>150000000</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>174960000</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>201840000</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>230640000</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>261360000</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>294000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:marker val="0"/>
         <c:smooth val="0"/>
         <c:axId val="511722003"/>
@@ -937,9 +1112,154 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="0"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:txPr>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1440000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2560000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7840000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10240000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12960000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19360000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23040000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27040000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31360000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46240000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51840000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57760000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70560000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84640000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>116640000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>134560000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>153760000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>174240000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>196000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
           <c:showLegendKey val="0"/>
           <c:showPercent val="0"/>
           <c:showSerName val="0"/>
@@ -1352,9 +1672,154 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2:$L$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="0"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:txPr>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>8640048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15360048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24000048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47040048</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61440048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77760048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116160048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>138240048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>162240048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>188160048</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>216000048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>277440048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>311040048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>346560048</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>423360048</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>507840048</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600000048</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>699840048</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>807360048</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>922560048</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1045440048</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1176000048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
           <c:showLegendKey val="0"/>
           <c:showPercent val="0"/>
           <c:showSerName val="0"/>
@@ -1763,6 +2228,149 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2:$M$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="0"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:txPr>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>10080000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17920000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54880000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71680000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90720000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135520000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>161280000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189280000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>219520000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>252000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>323680000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>362880000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>404320000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>493920000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>592480000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>700000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>816480000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>941920000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1076320000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1219680000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1372000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$23</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -2191,6 +2799,150 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$2:$J$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="0"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:txPr>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>105840000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>188160000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>294000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>576240000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>752640000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>952560000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1422960000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1693440000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1987440000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2304960000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2646000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3398640000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3810240000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4245360000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5186160000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6221040000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7350000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8573040000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9890160000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11301360000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12806640000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14406000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
@@ -2607,6 +3359,150 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2:$K$23</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="0"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:txPr>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>720000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1280000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3920000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5120000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6480000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9680000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11520000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13520000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15680000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25920000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28880000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35280000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42320000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58320000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>67280000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>76880000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>87120000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>98000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$23</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -6446,7 +7342,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>3174</xdr:rowOff>
+      <xdr:rowOff>3173</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -6478,13 +7374,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1525814</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>3174</xdr:rowOff>
+      <xdr:rowOff>3173</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>716642</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>171448</xdr:rowOff>
+      <xdr:rowOff>171447</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6574,7 +7470,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>171223</xdr:rowOff>
+      <xdr:rowOff>171222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -7093,7 +7989,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="E23" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="K4" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -7109,9 +8005,11 @@
     <col bestFit="1" min="10" max="10" width="15.3828125"/>
     <col bestFit="1" min="11" max="11" width="15.76171875"/>
     <col bestFit="1" min="12" max="13" width="11.19140625"/>
+    <col bestFit="1" min="15" max="16" width="13.8515625"/>
+    <col customWidth="1" min="17" max="17" width="15.140625"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="42.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7150,31 +8048,43 @@
       </c>
       <c r="M1" t="s">
         <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>600</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.001214</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>0.001531</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>0.0027079999999999999</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>0.0028839999999999998</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>0.037731000000000001</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <f t="shared" ref="H2:H9" si="0">(2*3)*B2*B2</f>
         <v>2160000</v>
       </c>
@@ -7196,27 +8106,43 @@
       <c r="M2">
         <v>10080000</v>
       </c>
+      <c r="O2" s="4">
+        <f t="shared" ref="O2:O9" si="4">0.0023+9.342e-11*H2+6.228e-11*I2</f>
+        <v>0.0025914704000000004</v>
+      </c>
+      <c r="P2" s="4">
+        <f t="shared" ref="P2:P9" si="5">0.005859876+1.297497e-11*J2+-7.920474e-11*K2</f>
+        <v>0.007176119412</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>0.001+2.288e-10*L2</f>
+        <v>0.0029768429823999998</v>
+      </c>
+      <c r="R2">
+        <f>0.001596489+2.400611e-10*M2</f>
+        <v>0.004016304888</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>800</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.001554</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>0.0026450000000000002</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>0.0043709999999999999</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>0.0047710000000000001</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>0.072558999999999998</v>
       </c>
       <c r="H3">
@@ -7241,27 +8167,43 @@
       <c r="M3">
         <v>17920000</v>
       </c>
+      <c r="O3" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0028181695999999999</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" si="5"/>
+        <v>0.008199864288</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>0.001+2.288e-10*L3</f>
+        <v>0.0045143789824000002</v>
+      </c>
+      <c r="R3" s="6">
+        <f>0.001596489+2.400611e-10*M3</f>
+        <v>0.0058983839119999999</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>1000</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>0.0023310000000000002</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>0.0056979999999999999</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>0.0062630000000000003</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>0.0071599999999999997</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>0.11128</v>
       </c>
       <c r="H4">
@@ -7286,27 +8228,43 @@
       <c r="M4">
         <v>28000000</v>
       </c>
+      <c r="O4" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0031096400000000003</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="5"/>
+        <v>0.0095161077</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>0.001+2.288e-10*L4</f>
+        <v>0.0064912109823999998</v>
+      </c>
+      <c r="R4" s="6">
+        <f>0.001596489+2.400611e-10*M4</f>
+        <v>0.0083181998000000004</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>1400</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>0.0035460000000000001</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>0.011006999999999999</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>0.011771</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>0.01388</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>0.19203899999999999</v>
       </c>
       <c r="H5">
@@ -7331,27 +8289,43 @@
       <c r="M5">
         <v>54880000</v>
       </c>
+      <c r="O5" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0038868943999999998</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="5"/>
+        <v>0.013026090132000002</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>0.001+2.288e-10*L5</f>
+        <v>0.011762762982400001</v>
+      </c>
+      <c r="R5" s="6">
+        <f>0.001596489+2.400611e-10*M5</f>
+        <v>0.014771042167999999</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>1600</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.0042570000000000004</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>0.014317</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>0.015017000000000001</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>0.017668</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>0.23905899999999999</v>
       </c>
       <c r="H6">
@@ -7376,27 +8350,43 @@
       <c r="M6">
         <v>71680000</v>
       </c>
+      <c r="O6" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0043726783999999998</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="5"/>
+        <v>0.015219829151999998</v>
+      </c>
+      <c r="Q6" s="5">
+        <f>0.001+2.288e-10*L6</f>
+        <v>0.015057482982399999</v>
+      </c>
+      <c r="R6" s="6">
+        <f>0.001596489+2.400611e-10*M6</f>
+        <v>0.018804068647999998</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>1800</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>0.0051130000000000004</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>0.018030000000000001</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>0.018711999999999999</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>0.021478000000000001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>0.28415099999999999</v>
       </c>
       <c r="H7">
@@ -7421,27 +8411,43 @@
       <c r="M7">
         <v>90720000</v>
       </c>
+      <c r="O7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0049232336000000002</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.017706066708000002</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>0.001+2.288e-10*L7</f>
+        <v>0.018791498982400002</v>
+      </c>
+      <c r="R7" s="6">
+        <f>0.001596489+2.400611e-10*M7</f>
+        <v>0.023374831991999998</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>2200</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>0.0070910000000000001</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>0.026831000000000001</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>0.027656</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>0.033416000000000001</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>0.39872099999999999</v>
       </c>
       <c r="H8">
@@ -7466,27 +8472,43 @@
       <c r="M8">
         <v>135520000</v>
       </c>
+      <c r="O8" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0062186576</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="5"/>
+        <v>0.023556037427999998</v>
+      </c>
+      <c r="Q8" s="5">
+        <f>0.001+2.288e-10*L8</f>
+        <v>0.027577418982400001</v>
+      </c>
+      <c r="R8" s="6">
+        <f>0.001596489+2.400611e-10*M8</f>
+        <v>0.034129569271999997</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>2400</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.0081689999999999992</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>0.031871999999999998</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>0.032870999999999997</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>0.041029999999999997</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>0.47762700000000002</v>
       </c>
       <c r="H9">
@@ -7511,43 +8533,59 @@
       <c r="M9">
         <v>161280000</v>
       </c>
+      <c r="O9" s="4">
+        <f t="shared" si="4"/>
+        <v>0.0069635263999999995</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="5"/>
+        <v>0.026919770592</v>
+      </c>
+      <c r="Q9" s="5">
+        <f>0.001+2.288e-10*L9</f>
+        <v>0.032629322982400004</v>
+      </c>
+      <c r="R9" s="6">
+        <f>0.001596489+2.400611e-10*M9</f>
+        <v>0.040313543207999999</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>2600</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>0.0094599999999999997</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>0.037366999999999997</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>0.038212999999999997</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>0.047203000000000002</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>0.55155100000000001</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H23" si="4">(2*3)*B10*B10</f>
+        <f t="shared" ref="H10:H23" si="6">(2*3)*B10*B10</f>
         <v>40560000</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I23" si="5">(1+(1*3))*B10*B10</f>
+        <f t="shared" ref="I10:I23" si="7">(1+(1*3))*B10*B10</f>
         <v>27040000</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10:J23" si="6">(7*7*(3+3))*B10*B10</f>
+        <f t="shared" ref="J10:J23" si="8">(7*7*(3+3))*B10*B10</f>
         <v>1987440000</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K23" si="7">(1+1)*B10*B10</f>
+        <f t="shared" ref="K10:K23" si="9">(1+1)*B10*B10</f>
         <v>13520000</v>
       </c>
       <c r="L10">
@@ -7555,44 +8593,60 @@
       </c>
       <c r="M10">
         <v>189280000</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" ref="O10:O23" si="10">0.0023+9.342e-11*H10+6.228e-11*I10</f>
+        <v>0.0077731663999999999</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" ref="P10:P23" si="11">0.005859876+1.297497e-11*J10+-7.920474e-11*K10</f>
+        <v>0.030576002291999999</v>
+      </c>
+      <c r="Q10" s="5">
+        <f>0.001+2.288e-10*L10</f>
+        <v>0.038120522982399999</v>
+      </c>
+      <c r="R10" s="6">
+        <f>0.001596489+2.400611e-10*M10</f>
+        <v>0.047035254007999995</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>2800</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>0.010655</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>0.043307999999999999</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>0.043642</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>0.052505000000000003</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>0.61951500000000004</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>47040000</v>
       </c>
       <c r="I11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>31360000</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2304960000</v>
       </c>
       <c r="K11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15680000</v>
       </c>
       <c r="L11">
@@ -7600,44 +8654,60 @@
       </c>
       <c r="M11">
         <v>219520000</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="10"/>
+        <v>0.0086475775999999994</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="11"/>
+        <v>0.034524732528000007</v>
+      </c>
+      <c r="Q11" s="5">
+        <f>0.001+2.288e-10*L11</f>
+        <v>0.044051018982399999</v>
+      </c>
+      <c r="R11" s="6">
+        <f>0.001596489+2.400611e-10*M11</f>
+        <v>0.054294701671999998</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>3000</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>0.01039</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>0.042139000000000003</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>0.050979999999999998</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>0.061419000000000001</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>0.78026600000000002</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>54000000</v>
       </c>
       <c r="I12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>36000000</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2646000000</v>
       </c>
       <c r="K12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>18000000</v>
       </c>
       <c r="L12">
@@ -7645,44 +8715,60 @@
       </c>
       <c r="M12">
         <v>252000000</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="10"/>
+        <v>0.0095867599999999997</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="11"/>
+        <v>0.038765961299999999</v>
+      </c>
+      <c r="Q12" s="5">
+        <f>0.001+2.288e-10*L12</f>
+        <v>0.050420810982399998</v>
+      </c>
+      <c r="R12" s="6">
+        <f>0.001596489+2.400611e-10*M12</f>
+        <v>0.062091886199999995</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>3400</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>0.012456999999999999</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>0.051378</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>0.064410999999999996</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>0.079176999999999997</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>0.97920799999999997</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>69360000</v>
       </c>
       <c r="I13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>46240000</v>
       </c>
       <c r="J13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3398640000</v>
       </c>
       <c r="K13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>23120000</v>
       </c>
       <c r="L13">
@@ -7690,44 +8776,60 @@
       </c>
       <c r="M13">
         <v>323680000</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="10"/>
+        <v>0.0116594384</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="11"/>
+        <v>0.048125914451999999</v>
+      </c>
+      <c r="Q13" s="5">
+        <f>0.001+2.288e-10*L13</f>
+        <v>0.064478282982400006</v>
+      </c>
+      <c r="R13" s="6">
+        <f>0.001596489+2.400611e-10*M13</f>
+        <v>0.079299465848000003</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>3600</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>0.012558</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>0.051908999999999997</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>0.072309999999999999</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>0.087878999999999999</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>1.1001510000000001</v>
       </c>
       <c r="H14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>77760000</v>
       </c>
       <c r="I14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>51840000</v>
       </c>
       <c r="J14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3810240000</v>
       </c>
       <c r="K14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>25920000</v>
       </c>
       <c r="L14">
@@ -7735,44 +8837,60 @@
       </c>
       <c r="M14">
         <v>362880000</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="10"/>
+        <v>0.012792934400000001</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="11"/>
+        <v>0.053244638832000001</v>
+      </c>
+      <c r="Q14" s="5">
+        <f>0.001+2.288e-10*L14</f>
+        <v>0.072165962982399995</v>
+      </c>
+      <c r="R14" s="6">
+        <f>0.001596489+2.400611e-10*M14</f>
+        <v>0.088709860968000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>3800</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>0.013145</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>0.055044999999999997</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>0.079882999999999996</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <v>0.099678000000000003</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>1.213042</v>
       </c>
       <c r="H15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>86640000</v>
       </c>
       <c r="I15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>57760000</v>
       </c>
       <c r="J15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4245360000</v>
       </c>
       <c r="K15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>28880000</v>
       </c>
       <c r="L15">
@@ -7780,44 +8898,60 @@
       </c>
       <c r="M15">
         <v>404320000</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="10"/>
+        <v>0.013991201600000001</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="11"/>
+        <v>0.058655861747999999</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>0.001+2.288e-10*L15</f>
+        <v>0.080292938982400003</v>
+      </c>
+      <c r="R15" s="6">
+        <f>0.001596489+2.400611e-10*M15</f>
+        <v>0.098657992952000007</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>4200</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>0.015831000000000001</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>0.067405000000000007</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2">
         <v>0.097278000000000003</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <v>0.119448</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <v>1.47638</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>105840000</v>
       </c>
       <c r="I16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>70560000</v>
       </c>
       <c r="J16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5186160000</v>
       </c>
       <c r="K16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>35280000</v>
       </c>
       <c r="L16">
@@ -7825,44 +8959,60 @@
       </c>
       <c r="M16">
         <v>493920000</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" si="10"/>
+        <v>0.016582049599999999</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" si="11"/>
+        <v>0.070355803187999999</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>0.001+2.288e-10*L16</f>
+        <v>0.097864778982400008</v>
+      </c>
+      <c r="R16" s="6">
+        <f>0.001596489+2.400611e-10*M16</f>
+        <v>0.120167467512</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>4600</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>0.018789</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>0.080714999999999995</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>0.116822</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <v>0.144928</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <v>1.733215</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>126960000</v>
       </c>
       <c r="I17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>84640000</v>
       </c>
       <c r="J17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6221040000</v>
       </c>
       <c r="K17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>42320000</v>
       </c>
       <c r="L17">
@@ -7870,44 +9020,60 @@
       </c>
       <c r="M17">
         <v>592480000</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" si="10"/>
+        <v>0.019431982399999999</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" si="11"/>
+        <v>0.083225738771999999</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>0.001+2.288e-10*L17</f>
+        <v>0.11719380298240001</v>
+      </c>
+      <c r="R17" s="6">
+        <f>0.001596489+2.400611e-10*M17</f>
+        <v>0.14382788952799999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>5000</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>0.022027000000000001</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>0.09511</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>0.14005100000000001</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <v>0.185276</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>2.092543</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>150000000</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100000000</v>
       </c>
       <c r="J18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7350000000</v>
       </c>
       <c r="K18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>50000000</v>
       </c>
       <c r="L18">
@@ -7915,44 +9081,60 @@
       </c>
       <c r="M18">
         <v>700000000</v>
+      </c>
+      <c r="O18" s="4">
+        <f t="shared" si="10"/>
+        <v>0.022541000000000002</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" si="11"/>
+        <v>0.097265668499999985</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>0.001+2.288e-10*L18</f>
+        <v>0.1382800109824</v>
+      </c>
+      <c r="R18" s="6">
+        <f>0.001596489+2.400611e-10*M18</f>
+        <v>0.16963925899999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>5400</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>0.025701000000000002</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <v>0.111294</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <v>0.15959999999999999</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <v>0.20069300000000001</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>2.3931520000000002</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>174960000</v>
       </c>
       <c r="I19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>116640000</v>
       </c>
       <c r="J19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8573040000</v>
       </c>
       <c r="K19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>58320000</v>
       </c>
       <c r="L19">
@@ -7960,44 +9142,60 @@
       </c>
       <c r="M19">
         <v>816480000</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="10"/>
+        <v>0.025909102400000002</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" si="11"/>
+        <v>0.11247559237199999</v>
+      </c>
+      <c r="Q19" s="5">
+        <f>0.001+2.288e-10*L19</f>
+        <v>0.16112340298239999</v>
+      </c>
+      <c r="R19" s="6">
+        <f>0.001596489+2.400611e-10*M19</f>
+        <v>0.19760157592799998</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>5800</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>0.029441999999999999</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="2">
         <v>0.128412</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2">
         <v>0.18646799999999999</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <v>0.23116</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>2.7512569999999998</v>
       </c>
       <c r="H20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>201840000</v>
       </c>
       <c r="I20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>134560000</v>
       </c>
       <c r="J20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9890160000</v>
       </c>
       <c r="K20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67280000</v>
       </c>
       <c r="L20">
@@ -8005,44 +9203,60 @@
       </c>
       <c r="M20">
         <v>941920000</v>
+      </c>
+      <c r="O20" s="4">
+        <f t="shared" si="10"/>
+        <v>0.029536289600000001</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" si="11"/>
+        <v>0.12885551038799997</v>
+      </c>
+      <c r="Q20" s="5">
+        <f>0.001+2.288e-10*L20</f>
+        <v>0.18572397898240001</v>
+      </c>
+      <c r="R20" s="6">
+        <f>0.001596489+2.400611e-10*M20</f>
+        <v>0.22771484031199998</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>6200</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>0.033391999999999998</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>0.146454</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
         <v>0.21267800000000001</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <v>0.26286700000000002</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <v>3.1154190000000002</v>
       </c>
       <c r="H21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>230640000</v>
       </c>
       <c r="I21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>153760000</v>
       </c>
       <c r="J21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>11301360000</v>
       </c>
       <c r="K21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>76880000</v>
       </c>
       <c r="L21">
@@ -8050,44 +9264,60 @@
       </c>
       <c r="M21">
         <v>1076320000</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="10"/>
+        <v>0.033422561599999998</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="11"/>
+        <v>0.14640542254799999</v>
+      </c>
+      <c r="Q21" s="5">
+        <f>0.001+2.288e-10*L21</f>
+        <v>0.21208173898240001</v>
+      </c>
+      <c r="R21" s="6">
+        <f>0.001596489+2.400611e-10*M21</f>
+        <v>0.25997905215199996</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>6600</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>0.037482000000000001</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>0.16541800000000001</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="2">
         <v>0.24410200000000001</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="2">
         <v>0.27819500000000003</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <v>3.5119750000000001</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>261360000</v>
       </c>
       <c r="I22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>174240000</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12806640000</v>
       </c>
       <c r="K22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>87120000</v>
       </c>
       <c r="L22">
@@ -8095,44 +9325,60 @@
       </c>
       <c r="M22">
         <v>1219680000</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="10"/>
+        <v>0.037567918399999997</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="11"/>
+        <v>0.16512532885199999</v>
+      </c>
+      <c r="Q22" s="5">
+        <f>0.001+2.288e-10*L22</f>
+        <v>0.24019668298239999</v>
+      </c>
+      <c r="R22" s="6">
+        <f>0.001596489+2.400611e-10*M22</f>
+        <v>0.29439421144799999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>7000</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>0.042598999999999998</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="2">
         <v>0.186052</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2">
         <v>0.26590399999999997</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="2">
         <v>0.331285</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2">
         <v>3.960623</v>
       </c>
       <c r="H23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>294000000</v>
       </c>
       <c r="I23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>196000000</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14406000000</v>
       </c>
       <c r="K23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>98000000</v>
       </c>
       <c r="L23">
@@ -8141,24 +9387,43 @@
       <c r="M23">
         <v>1372000000</v>
       </c>
+      <c r="O23" s="4">
+        <f t="shared" si="10"/>
+        <v>0.04197236</v>
+      </c>
+      <c r="P23" s="4">
+        <f t="shared" si="11"/>
+        <v>0.18501522929999997</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>0.001+2.288e-10*L23</f>
+        <v>0.27006881098239999</v>
+      </c>
+      <c r="R23" s="6">
+        <f>0.001596489+2.400611e-10*M23</f>
+        <v>0.33096031819999994</v>
+      </c>
     </row>
-    <row r="24"/>
+    <row r="24">
+      <c r="Q24" s="5"/>
+    </row>
     <row r="25" ht="26.25">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="4"/>
+      <c r="A25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="Q25" s="5"/>
     </row>
     <row r="26"/>
     <row r="27" ht="14.25"/>

</xml_diff>

<commit_message>
Add more data to xlsx
</commit_message>
<xml_diff>
--- a/Assignments/PA4/training.xlsx
+++ b/Assignments/PA4/training.xlsx
@@ -2260,6 +2260,7 @@
           <c:dLbls>
             <c:showBubbleSize val="0"/>
             <c:showCatName val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:showLegendKey val="0"/>
             <c:showPercent val="0"/>
             <c:showSerName val="0"/>
@@ -7989,7 +7990,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="K4" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8082,7 +8083,8 @@
         <v>0.0028839999999999998</v>
       </c>
       <c r="G2" s="2">
-        <v>0.037731000000000001</v>
+        <f>SUM(C2:F2)</f>
+        <v>0.0083369999999999989</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ref="H2:H9" si="0">(2*3)*B2*B2</f>
@@ -8101,9 +8103,11 @@
         <v>720000</v>
       </c>
       <c r="L2">
+        <f>(4*(B2*B2*4)+3*4*4)+2*(B2*B2*4)</f>
         <v>8640048</v>
       </c>
       <c r="M2">
+        <f>4*(4*B2*B2)+(B2*B2*3*4)</f>
         <v>10080000</v>
       </c>
       <c r="O2" s="4">
@@ -8115,11 +8119,11 @@
         <v>0.007176119412</v>
       </c>
       <c r="Q2" s="5">
-        <f>0.001+2.288e-10*L2</f>
+        <f t="shared" ref="Q2:Q9" si="6">0.001+2.288e-10*L2</f>
         <v>0.0029768429823999998</v>
       </c>
       <c r="R2">
-        <f>0.001596489+2.400611e-10*M2</f>
+        <f t="shared" ref="R2:R9" si="7">0.001596489+2.400611e-10*M2</f>
         <v>0.004016304888</v>
       </c>
     </row>
@@ -8143,7 +8147,8 @@
         <v>0.0047710000000000001</v>
       </c>
       <c r="G3" s="2">
-        <v>0.072558999999999998</v>
+        <f>SUM(C3:F3)</f>
+        <v>0.013341000000000002</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
@@ -8162,9 +8167,11 @@
         <v>1280000</v>
       </c>
       <c r="L3">
+        <f>(4*(B3*B3*4)+3*4*4)+2*(B3*B3*4)</f>
         <v>15360048</v>
       </c>
       <c r="M3">
+        <f>4*(4*B3*B3)+(B3*B3*3*4)</f>
         <v>17920000</v>
       </c>
       <c r="O3" s="4">
@@ -8176,11 +8183,11 @@
         <v>0.008199864288</v>
       </c>
       <c r="Q3" s="5">
-        <f>0.001+2.288e-10*L3</f>
+        <f t="shared" si="6"/>
         <v>0.0045143789824000002</v>
       </c>
       <c r="R3" s="6">
-        <f>0.001596489+2.400611e-10*M3</f>
+        <f t="shared" si="7"/>
         <v>0.0058983839119999999</v>
       </c>
     </row>
@@ -8204,7 +8211,8 @@
         <v>0.0071599999999999997</v>
       </c>
       <c r="G4" s="2">
-        <v>0.11128</v>
+        <f>SUM(C4:F4)</f>
+        <v>0.021451999999999999</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -8223,9 +8231,11 @@
         <v>2000000</v>
       </c>
       <c r="L4">
+        <f>(4*(B4*B4*4)+3*4*4)+2*(B4*B4*4)</f>
         <v>24000048</v>
       </c>
       <c r="M4">
+        <f>4*(4*B4*B4)+(B4*B4*3*4)</f>
         <v>28000000</v>
       </c>
       <c r="O4" s="4">
@@ -8237,11 +8247,11 @@
         <v>0.0095161077</v>
       </c>
       <c r="Q4" s="5">
-        <f>0.001+2.288e-10*L4</f>
+        <f t="shared" si="6"/>
         <v>0.0064912109823999998</v>
       </c>
       <c r="R4" s="6">
-        <f>0.001596489+2.400611e-10*M4</f>
+        <f t="shared" si="7"/>
         <v>0.0083181998000000004</v>
       </c>
     </row>
@@ -8265,7 +8275,8 @@
         <v>0.01388</v>
       </c>
       <c r="G5" s="2">
-        <v>0.19203899999999999</v>
+        <f>SUM(C5:F5)</f>
+        <v>0.040204000000000004</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -8284,9 +8295,11 @@
         <v>3920000</v>
       </c>
       <c r="L5">
+        <f>(4*(B5*B5*4)+3*4*4)+2*(B5*B5*4)</f>
         <v>47040048</v>
       </c>
       <c r="M5">
+        <f>4*(4*B5*B5)+(B5*B5*3*4)</f>
         <v>54880000</v>
       </c>
       <c r="O5" s="4">
@@ -8298,11 +8311,11 @@
         <v>0.013026090132000002</v>
       </c>
       <c r="Q5" s="5">
-        <f>0.001+2.288e-10*L5</f>
+        <f t="shared" si="6"/>
         <v>0.011762762982400001</v>
       </c>
       <c r="R5" s="6">
-        <f>0.001596489+2.400611e-10*M5</f>
+        <f t="shared" si="7"/>
         <v>0.014771042167999999</v>
       </c>
     </row>
@@ -8326,7 +8339,8 @@
         <v>0.017668</v>
       </c>
       <c r="G6" s="2">
-        <v>0.23905899999999999</v>
+        <f>SUM(C6:F6)</f>
+        <v>0.051258999999999999</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -8345,9 +8359,11 @@
         <v>5120000</v>
       </c>
       <c r="L6">
+        <f>(4*(B6*B6*4)+3*4*4)+2*(B6*B6*4)</f>
         <v>61440048</v>
       </c>
       <c r="M6">
+        <f>4*(4*B6*B6)+(B6*B6*3*4)</f>
         <v>71680000</v>
       </c>
       <c r="O6" s="4">
@@ -8359,11 +8375,11 @@
         <v>0.015219829151999998</v>
       </c>
       <c r="Q6" s="5">
-        <f>0.001+2.288e-10*L6</f>
+        <f t="shared" si="6"/>
         <v>0.015057482982399999</v>
       </c>
       <c r="R6" s="6">
-        <f>0.001596489+2.400611e-10*M6</f>
+        <f t="shared" si="7"/>
         <v>0.018804068647999998</v>
       </c>
     </row>
@@ -8387,7 +8403,8 @@
         <v>0.021478000000000001</v>
       </c>
       <c r="G7" s="2">
-        <v>0.28415099999999999</v>
+        <f>SUM(C7:F7)</f>
+        <v>0.063333</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
@@ -8406,9 +8423,11 @@
         <v>6480000</v>
       </c>
       <c r="L7">
+        <f>(4*(B7*B7*4)+3*4*4)+2*(B7*B7*4)</f>
         <v>77760048</v>
       </c>
       <c r="M7">
+        <f>4*(4*B7*B7)+(B7*B7*3*4)</f>
         <v>90720000</v>
       </c>
       <c r="O7" s="4">
@@ -8420,11 +8439,11 @@
         <v>0.017706066708000002</v>
       </c>
       <c r="Q7" s="5">
-        <f>0.001+2.288e-10*L7</f>
+        <f t="shared" si="6"/>
         <v>0.018791498982400002</v>
       </c>
       <c r="R7" s="6">
-        <f>0.001596489+2.400611e-10*M7</f>
+        <f t="shared" si="7"/>
         <v>0.023374831991999998</v>
       </c>
     </row>
@@ -8448,7 +8467,8 @@
         <v>0.033416000000000001</v>
       </c>
       <c r="G8" s="2">
-        <v>0.39872099999999999</v>
+        <f>SUM(C8:F8)</f>
+        <v>0.094993999999999995</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -8467,9 +8487,11 @@
         <v>9680000</v>
       </c>
       <c r="L8">
+        <f>(4*(B8*B8*4)+3*4*4)+2*(B8*B8*4)</f>
         <v>116160048</v>
       </c>
       <c r="M8">
+        <f>4*(4*B8*B8)+(B8*B8*3*4)</f>
         <v>135520000</v>
       </c>
       <c r="O8" s="4">
@@ -8481,11 +8503,11 @@
         <v>0.023556037427999998</v>
       </c>
       <c r="Q8" s="5">
-        <f>0.001+2.288e-10*L8</f>
+        <f t="shared" si="6"/>
         <v>0.027577418982400001</v>
       </c>
       <c r="R8" s="6">
-        <f>0.001596489+2.400611e-10*M8</f>
+        <f t="shared" si="7"/>
         <v>0.034129569271999997</v>
       </c>
     </row>
@@ -8509,7 +8531,8 @@
         <v>0.041029999999999997</v>
       </c>
       <c r="G9" s="2">
-        <v>0.47762700000000002</v>
+        <f>SUM(C9:F9)</f>
+        <v>0.11394199999999999</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
@@ -8528,9 +8551,11 @@
         <v>11520000</v>
       </c>
       <c r="L9">
+        <f>(4*(B9*B9*4)+3*4*4)+2*(B9*B9*4)</f>
         <v>138240048</v>
       </c>
       <c r="M9">
+        <f>4*(4*B9*B9)+(B9*B9*3*4)</f>
         <v>161280000</v>
       </c>
       <c r="O9" s="4">
@@ -8542,11 +8567,11 @@
         <v>0.026919770592</v>
       </c>
       <c r="Q9" s="5">
-        <f>0.001+2.288e-10*L9</f>
+        <f t="shared" si="6"/>
         <v>0.032629322982400004</v>
       </c>
       <c r="R9" s="6">
-        <f>0.001596489+2.400611e-10*M9</f>
+        <f t="shared" si="7"/>
         <v>0.040313543207999999</v>
       </c>
     </row>
@@ -8570,44 +8595,47 @@
         <v>0.047203000000000002</v>
       </c>
       <c r="G10" s="2">
-        <v>0.55155100000000001</v>
+        <f>SUM(C10:F10)</f>
+        <v>0.132243</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H23" si="6">(2*3)*B10*B10</f>
+        <f t="shared" ref="H10:H23" si="8">(2*3)*B10*B10</f>
         <v>40560000</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I23" si="7">(1+(1*3))*B10*B10</f>
+        <f t="shared" ref="I10:I23" si="9">(1+(1*3))*B10*B10</f>
         <v>27040000</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10:J23" si="8">(7*7*(3+3))*B10*B10</f>
+        <f t="shared" ref="J10:J23" si="10">(7*7*(3+3))*B10*B10</f>
         <v>1987440000</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K23" si="9">(1+1)*B10*B10</f>
+        <f t="shared" ref="K10:K23" si="11">(1+1)*B10*B10</f>
         <v>13520000</v>
       </c>
       <c r="L10">
+        <f>(4*(B10*B10*4)+3*4*4)+2*(B10*B10*4)</f>
         <v>162240048</v>
       </c>
       <c r="M10">
+        <f>4*(4*B10*B10)+(B10*B10*3*4)</f>
         <v>189280000</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" ref="O10:O23" si="10">0.0023+9.342e-11*H10+6.228e-11*I10</f>
+        <f t="shared" ref="O10:O23" si="12">0.0023+9.342e-11*H10+6.228e-11*I10</f>
         <v>0.0077731663999999999</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" ref="P10:P23" si="11">0.005859876+1.297497e-11*J10+-7.920474e-11*K10</f>
+        <f t="shared" ref="P10:P23" si="13">0.005859876+1.297497e-11*J10+-7.920474e-11*K10</f>
         <v>0.030576002291999999</v>
       </c>
       <c r="Q10" s="5">
-        <f>0.001+2.288e-10*L10</f>
+        <f t="shared" ref="Q10:Q23" si="14">0.001+2.288e-10*L10</f>
         <v>0.038120522982399999</v>
       </c>
       <c r="R10" s="6">
-        <f>0.001596489+2.400611e-10*M10</f>
+        <f t="shared" ref="R10:R23" si="15">0.001596489+2.400611e-10*M10</f>
         <v>0.047035254007999995</v>
       </c>
     </row>
@@ -8631,44 +8659,47 @@
         <v>0.052505000000000003</v>
       </c>
       <c r="G11" s="2">
-        <v>0.61951500000000004</v>
+        <f>SUM(C11:F11)</f>
+        <v>0.15010999999999999</v>
       </c>
       <c r="H11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>47040000</v>
       </c>
       <c r="I11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>31360000</v>
       </c>
       <c r="J11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2304960000</v>
       </c>
       <c r="K11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>15680000</v>
       </c>
       <c r="L11">
+        <f>(4*(B11*B11*4)+3*4*4)+2*(B11*B11*4)</f>
         <v>188160048</v>
       </c>
       <c r="M11">
+        <f>4*(4*B11*B11)+(B11*B11*3*4)</f>
         <v>219520000</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.0086475775999999994</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.034524732528000007</v>
       </c>
       <c r="Q11" s="5">
-        <f>0.001+2.288e-10*L11</f>
+        <f t="shared" si="14"/>
         <v>0.044051018982399999</v>
       </c>
       <c r="R11" s="6">
-        <f>0.001596489+2.400611e-10*M11</f>
+        <f t="shared" si="15"/>
         <v>0.054294701671999998</v>
       </c>
     </row>
@@ -8692,44 +8723,47 @@
         <v>0.061419000000000001</v>
       </c>
       <c r="G12" s="2">
-        <v>0.78026600000000002</v>
+        <f>SUM(C12:F12)</f>
+        <v>0.16492800000000002</v>
       </c>
       <c r="H12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>54000000</v>
       </c>
       <c r="I12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>36000000</v>
       </c>
       <c r="J12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2646000000</v>
       </c>
       <c r="K12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>18000000</v>
       </c>
       <c r="L12">
+        <f>(4*(B12*B12*4)+3*4*4)+2*(B12*B12*4)</f>
         <v>216000048</v>
       </c>
       <c r="M12">
+        <f>4*(4*B12*B12)+(B12*B12*3*4)</f>
         <v>252000000</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.0095867599999999997</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.038765961299999999</v>
       </c>
       <c r="Q12" s="5">
-        <f>0.001+2.288e-10*L12</f>
+        <f t="shared" si="14"/>
         <v>0.050420810982399998</v>
       </c>
       <c r="R12" s="6">
-        <f>0.001596489+2.400611e-10*M12</f>
+        <f t="shared" si="15"/>
         <v>0.062091886199999995</v>
       </c>
     </row>
@@ -8753,44 +8787,47 @@
         <v>0.079176999999999997</v>
       </c>
       <c r="G13" s="2">
-        <v>0.97920799999999997</v>
+        <f>SUM(C13:F13)</f>
+        <v>0.207423</v>
       </c>
       <c r="H13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>69360000</v>
       </c>
       <c r="I13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>46240000</v>
       </c>
       <c r="J13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3398640000</v>
       </c>
       <c r="K13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>23120000</v>
       </c>
       <c r="L13">
+        <f>(4*(B13*B13*4)+3*4*4)+2*(B13*B13*4)</f>
         <v>277440048</v>
       </c>
       <c r="M13">
+        <f>4*(4*B13*B13)+(B13*B13*3*4)</f>
         <v>323680000</v>
       </c>
       <c r="O13" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.0116594384</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.048125914451999999</v>
       </c>
       <c r="Q13" s="5">
-        <f>0.001+2.288e-10*L13</f>
+        <f t="shared" si="14"/>
         <v>0.064478282982400006</v>
       </c>
       <c r="R13" s="6">
-        <f>0.001596489+2.400611e-10*M13</f>
+        <f t="shared" si="15"/>
         <v>0.079299465848000003</v>
       </c>
     </row>
@@ -8814,44 +8851,47 @@
         <v>0.087878999999999999</v>
       </c>
       <c r="G14" s="2">
-        <v>1.1001510000000001</v>
+        <f>SUM(C14:F14)</f>
+        <v>0.22465599999999997</v>
       </c>
       <c r="H14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>77760000</v>
       </c>
       <c r="I14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>51840000</v>
       </c>
       <c r="J14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3810240000</v>
       </c>
       <c r="K14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>25920000</v>
       </c>
       <c r="L14">
+        <f>(4*(B14*B14*4)+3*4*4)+2*(B14*B14*4)</f>
         <v>311040048</v>
       </c>
       <c r="M14">
+        <f>4*(4*B14*B14)+(B14*B14*3*4)</f>
         <v>362880000</v>
       </c>
       <c r="O14" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.012792934400000001</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.053244638832000001</v>
       </c>
       <c r="Q14" s="5">
-        <f>0.001+2.288e-10*L14</f>
+        <f t="shared" si="14"/>
         <v>0.072165962982399995</v>
       </c>
       <c r="R14" s="6">
-        <f>0.001596489+2.400611e-10*M14</f>
+        <f t="shared" si="15"/>
         <v>0.088709860968000001</v>
       </c>
     </row>
@@ -8875,44 +8915,47 @@
         <v>0.099678000000000003</v>
       </c>
       <c r="G15" s="2">
-        <v>1.213042</v>
+        <f>SUM(C15:F15)</f>
+        <v>0.247751</v>
       </c>
       <c r="H15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>86640000</v>
       </c>
       <c r="I15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>57760000</v>
       </c>
       <c r="J15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4245360000</v>
       </c>
       <c r="K15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>28880000</v>
       </c>
       <c r="L15">
+        <f>(4*(B15*B15*4)+3*4*4)+2*(B15*B15*4)</f>
         <v>346560048</v>
       </c>
       <c r="M15">
+        <f>4*(4*B15*B15)+(B15*B15*3*4)</f>
         <v>404320000</v>
       </c>
       <c r="O15" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.013991201600000001</v>
       </c>
       <c r="P15" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.058655861747999999</v>
       </c>
       <c r="Q15" s="5">
-        <f>0.001+2.288e-10*L15</f>
+        <f t="shared" si="14"/>
         <v>0.080292938982400003</v>
       </c>
       <c r="R15" s="6">
-        <f>0.001596489+2.400611e-10*M15</f>
+        <f t="shared" si="15"/>
         <v>0.098657992952000007</v>
       </c>
     </row>
@@ -8936,44 +8979,47 @@
         <v>0.119448</v>
       </c>
       <c r="G16" s="2">
-        <v>1.47638</v>
+        <f>SUM(C16:F16)</f>
+        <v>0.29996200000000001</v>
       </c>
       <c r="H16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>105840000</v>
       </c>
       <c r="I16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>70560000</v>
       </c>
       <c r="J16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5186160000</v>
       </c>
       <c r="K16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>35280000</v>
       </c>
       <c r="L16">
+        <f>(4*(B16*B16*4)+3*4*4)+2*(B16*B16*4)</f>
         <v>423360048</v>
       </c>
       <c r="M16">
+        <f>4*(4*B16*B16)+(B16*B16*3*4)</f>
         <v>493920000</v>
       </c>
       <c r="O16" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.016582049599999999</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.070355803187999999</v>
       </c>
       <c r="Q16" s="5">
-        <f>0.001+2.288e-10*L16</f>
+        <f t="shared" si="14"/>
         <v>0.097864778982400008</v>
       </c>
       <c r="R16" s="6">
-        <f>0.001596489+2.400611e-10*M16</f>
+        <f t="shared" si="15"/>
         <v>0.120167467512</v>
       </c>
     </row>
@@ -8997,44 +9043,47 @@
         <v>0.144928</v>
       </c>
       <c r="G17" s="2">
-        <v>1.733215</v>
+        <f>SUM(C17:F17)</f>
+        <v>0.36125399999999996</v>
       </c>
       <c r="H17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>126960000</v>
       </c>
       <c r="I17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>84640000</v>
       </c>
       <c r="J17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6221040000</v>
       </c>
       <c r="K17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>42320000</v>
       </c>
       <c r="L17">
+        <f>(4*(B17*B17*4)+3*4*4)+2*(B17*B17*4)</f>
         <v>507840048</v>
       </c>
       <c r="M17">
+        <f>4*(4*B17*B17)+(B17*B17*3*4)</f>
         <v>592480000</v>
       </c>
       <c r="O17" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.019431982399999999</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.083225738771999999</v>
       </c>
       <c r="Q17" s="5">
-        <f>0.001+2.288e-10*L17</f>
+        <f t="shared" si="14"/>
         <v>0.11719380298240001</v>
       </c>
       <c r="R17" s="6">
-        <f>0.001596489+2.400611e-10*M17</f>
+        <f t="shared" si="15"/>
         <v>0.14382788952799999</v>
       </c>
     </row>
@@ -9058,44 +9107,47 @@
         <v>0.185276</v>
       </c>
       <c r="G18" s="2">
-        <v>2.092543</v>
+        <f>SUM(C18:F18)</f>
+        <v>0.44246400000000002</v>
       </c>
       <c r="H18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>150000000</v>
       </c>
       <c r="I18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100000000</v>
       </c>
       <c r="J18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7350000000</v>
       </c>
       <c r="K18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>50000000</v>
       </c>
       <c r="L18">
+        <f>(4*(B18*B18*4)+3*4*4)+2*(B18*B18*4)</f>
         <v>600000048</v>
       </c>
       <c r="M18">
+        <f>4*(4*B18*B18)+(B18*B18*3*4)</f>
         <v>700000000</v>
       </c>
       <c r="O18" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.022541000000000002</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.097265668499999985</v>
       </c>
       <c r="Q18" s="5">
-        <f>0.001+2.288e-10*L18</f>
+        <f t="shared" si="14"/>
         <v>0.1382800109824</v>
       </c>
       <c r="R18" s="6">
-        <f>0.001596489+2.400611e-10*M18</f>
+        <f t="shared" si="15"/>
         <v>0.16963925899999999</v>
       </c>
     </row>
@@ -9119,44 +9171,47 @@
         <v>0.20069300000000001</v>
       </c>
       <c r="G19" s="2">
-        <v>2.3931520000000002</v>
+        <f>SUM(C19:F19)</f>
+        <v>0.49728800000000001</v>
       </c>
       <c r="H19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>174960000</v>
       </c>
       <c r="I19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>116640000</v>
       </c>
       <c r="J19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8573040000</v>
       </c>
       <c r="K19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>58320000</v>
       </c>
       <c r="L19">
+        <f>(4*(B19*B19*4)+3*4*4)+2*(B19*B19*4)</f>
         <v>699840048</v>
       </c>
       <c r="M19">
+        <f>4*(4*B19*B19)+(B19*B19*3*4)</f>
         <v>816480000</v>
       </c>
       <c r="O19" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.025909102400000002</v>
       </c>
       <c r="P19" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.11247559237199999</v>
       </c>
       <c r="Q19" s="5">
-        <f>0.001+2.288e-10*L19</f>
+        <f t="shared" si="14"/>
         <v>0.16112340298239999</v>
       </c>
       <c r="R19" s="6">
-        <f>0.001596489+2.400611e-10*M19</f>
+        <f t="shared" si="15"/>
         <v>0.19760157592799998</v>
       </c>
     </row>
@@ -9180,44 +9235,47 @@
         <v>0.23116</v>
       </c>
       <c r="G20" s="2">
-        <v>2.7512569999999998</v>
+        <f>SUM(C20:F20)</f>
+        <v>0.57548200000000005</v>
       </c>
       <c r="H20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>201840000</v>
       </c>
       <c r="I20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>134560000</v>
       </c>
       <c r="J20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9890160000</v>
       </c>
       <c r="K20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>67280000</v>
       </c>
       <c r="L20">
+        <f>(4*(B20*B20*4)+3*4*4)+2*(B20*B20*4)</f>
         <v>807360048</v>
       </c>
       <c r="M20">
+        <f>4*(4*B20*B20)+(B20*B20*3*4)</f>
         <v>941920000</v>
       </c>
       <c r="O20" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.029536289600000001</v>
       </c>
       <c r="P20" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.12885551038799997</v>
       </c>
       <c r="Q20" s="5">
-        <f>0.001+2.288e-10*L20</f>
+        <f t="shared" si="14"/>
         <v>0.18572397898240001</v>
       </c>
       <c r="R20" s="6">
-        <f>0.001596489+2.400611e-10*M20</f>
+        <f t="shared" si="15"/>
         <v>0.22771484031199998</v>
       </c>
     </row>
@@ -9241,44 +9299,47 @@
         <v>0.26286700000000002</v>
       </c>
       <c r="G21" s="2">
-        <v>3.1154190000000002</v>
+        <f>SUM(C21:F21)</f>
+        <v>0.65539100000000006</v>
       </c>
       <c r="H21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>230640000</v>
       </c>
       <c r="I21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>153760000</v>
       </c>
       <c r="J21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>11301360000</v>
       </c>
       <c r="K21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>76880000</v>
       </c>
       <c r="L21">
+        <f>(4*(B21*B21*4)+3*4*4)+2*(B21*B21*4)</f>
         <v>922560048</v>
       </c>
       <c r="M21">
+        <f>4*(4*B21*B21)+(B21*B21*3*4)</f>
         <v>1076320000</v>
       </c>
       <c r="O21" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.033422561599999998</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.14640542254799999</v>
       </c>
       <c r="Q21" s="5">
-        <f>0.001+2.288e-10*L21</f>
+        <f t="shared" si="14"/>
         <v>0.21208173898240001</v>
       </c>
       <c r="R21" s="6">
-        <f>0.001596489+2.400611e-10*M21</f>
+        <f t="shared" si="15"/>
         <v>0.25997905215199996</v>
       </c>
     </row>
@@ -9302,44 +9363,47 @@
         <v>0.27819500000000003</v>
       </c>
       <c r="G22" s="2">
-        <v>3.5119750000000001</v>
+        <f>SUM(C22:F22)</f>
+        <v>0.72519700000000009</v>
       </c>
       <c r="H22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>261360000</v>
       </c>
       <c r="I22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>174240000</v>
       </c>
       <c r="J22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12806640000</v>
       </c>
       <c r="K22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>87120000</v>
       </c>
       <c r="L22">
+        <f>(4*(B22*B22*4)+3*4*4)+2*(B22*B22*4)</f>
         <v>1045440048</v>
       </c>
       <c r="M22">
+        <f>4*(4*B22*B22)+(B22*B22*3*4)</f>
         <v>1219680000</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.037567918399999997</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.16512532885199999</v>
       </c>
       <c r="Q22" s="5">
-        <f>0.001+2.288e-10*L22</f>
+        <f t="shared" si="14"/>
         <v>0.24019668298239999</v>
       </c>
       <c r="R22" s="6">
-        <f>0.001596489+2.400611e-10*M22</f>
+        <f t="shared" si="15"/>
         <v>0.29439421144799999</v>
       </c>
     </row>
@@ -9363,44 +9427,47 @@
         <v>0.331285</v>
       </c>
       <c r="G23" s="2">
-        <v>3.960623</v>
+        <f>SUM(C23:F23)</f>
+        <v>0.82583999999999991</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>294000000</v>
       </c>
       <c r="I23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>196000000</v>
       </c>
       <c r="J23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>14406000000</v>
       </c>
       <c r="K23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>98000000</v>
       </c>
       <c r="L23">
+        <f>(4*(B23*B23*4)+3*4*4)+2*(B23*B23*4)</f>
         <v>1176000048</v>
       </c>
       <c r="M23">
+        <f>4*(4*B23*B23)+(B23*B23*3*4)</f>
         <v>1372000000</v>
       </c>
       <c r="O23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.04197236</v>
       </c>
       <c r="P23" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.18501522929999997</v>
       </c>
       <c r="Q23" s="5">
-        <f>0.001+2.288e-10*L23</f>
+        <f t="shared" si="14"/>
         <v>0.27006881098239999</v>
       </c>
       <c r="R23" s="6">
-        <f>0.001596489+2.400611e-10*M23</f>
+        <f t="shared" si="15"/>
         <v>0.33096031819999994</v>
       </c>
     </row>
@@ -9427,6 +9494,7 @@
     </row>
     <row r="26"/>
     <row r="27" ht="14.25"/>
+    <row r="29" ht="14.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A25:L25"/>

</xml_diff>